<commit_message>
[Added][Documentation] Added a Readme.md file, updated the path to results fileand made a first run
</commit_message>
<xml_diff>
--- a/Input files/NatureTool_Input_File_Template.xlsx
+++ b/Input files/NatureTool_Input_File_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itscdcbiodiversite-my.sharepoint.com/personal/marie_kovalenko_cdc-biodiversite_fr/Documents/Documents/GitHub/NatureTool/Input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_F25DC773A252ABDACC1048B4995E710C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BE1992B-7B27-4261-BF5F-577E3CF6F213}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC1048B4995E710C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5421FEBD-5562-46D3-9EAD-E515C65AFC88}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>ISIN</t>
   </si>
@@ -61,9 +61,6 @@
     <t>CH0012335540</t>
   </si>
   <si>
-    <t>GB00BP6MXD84</t>
-  </si>
-  <si>
     <t>GB00BYN59130</t>
   </si>
   <si>
@@ -86,13 +83,86 @@
   </si>
   <si>
     <t>CZ0005134601</t>
+  </si>
+  <si>
+    <t>NATURE TOOL INPUT FILE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please fill in the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"Input_data" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sheet before running the NatureTool</t>
+    </r>
+  </si>
+  <si>
+    <t>Input_data</t>
+  </si>
+  <si>
+    <t>Portfolio_name</t>
+  </si>
+  <si>
+    <t>Name of your portfolio (can be the same for all lines)</t>
+  </si>
+  <si>
+    <t>ISIN number in the portfolio</t>
+  </si>
+  <si>
+    <t>Invested amount related to the ISIN (equity or bond)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Currency of the amount. The list of authorized currencies is defined in the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Currency"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet</t>
+    </r>
+  </si>
+  <si>
+    <t>GB00BDCPN049</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +178,57 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,16 +236,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard_Blad1" xfId="1" xr:uid="{3C459817-4E24-49A5-AF78-6AC0F013B1F0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -422,12 +554,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{992CDB7D-C2ED-46E1-B2C5-73B8626643CD}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -440,7 +627,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,10 +645,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -475,7 +662,7 @@
         <v>4600000</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -489,7 +676,7 @@
         <v>7890000</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -503,21 +690,21 @@
         <v>59000</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C5">
         <v>5609800</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -525,13 +712,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1289000</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -539,13 +726,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>33000</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -580,22 +767,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Input file][Changed] changed the input file composition to avoid missing NACE codes, and uploading the associated new results file
</commit_message>
<xml_diff>
--- a/Input files/NatureTool_Input_File_Template.xlsx
+++ b/Input files/NatureTool_Input_File_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itscdcbiodiversite-my.sharepoint.com/personal/marie_kovalenko_cdc-biodiversite_fr/Documents/Documents/GitHub/NatureTool/Input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_F25DC773A252ABDACC1048B4995E710C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5421FEBD-5562-46D3-9EAD-E515C65AFC88}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_F25DC773A252ABDACC1048B4995E710C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EF3F04B-5A19-42A7-B31C-15DA920C9D9C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -236,33 +236,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,7 +611,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,7 +681,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5">

</xml_diff>